<commit_message>
second update of tool
</commit_message>
<xml_diff>
--- a/public/herramienta.xlsx
+++ b/public/herramienta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\OneDrive\Documentos\Proyectos\Frontend\pry20232028\diagnostic-tool\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEEC9BB-98E3-4307-BF5E-7092356D7F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0D81ED-B020-4ACA-918D-2E41515AF6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="891" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="891" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Caratula" sheetId="1" r:id="rId1"/>
@@ -13869,7 +13869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="55" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -17474,7 +17474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEC1250-B59F-4A52-8196-CD13BECFF42C}">
   <dimension ref="B2:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -17949,7 +17949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1262A127-4DF6-4F4F-B8F9-B35F9ACD5893}">
   <dimension ref="B2:J11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F6" sqref="E6:F6"/>
     </sheetView>
   </sheetViews>
@@ -18540,7 +18540,7 @@
   <dimension ref="B2:J31"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
adding fonticons, authors and description for index.astro
</commit_message>
<xml_diff>
--- a/public/herramienta.xlsx
+++ b/public/herramienta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\OneDrive\Documentos\Proyectos\Frontend\pry20232028\diagnostic-tool\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0D81ED-B020-4ACA-918D-2E41515AF6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476B81F-7A28-4992-8E6B-7FC03D261ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="891" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="451">
   <si>
     <t xml:space="preserve">
 </t>
@@ -1478,6 +1478,36 @@
   </si>
   <si>
     <t>FASE</t>
+  </si>
+  <si>
+    <t>[0</t>
+  </si>
+  <si>
+    <t>0.2&gt;</t>
+  </si>
+  <si>
+    <t>[0.2</t>
+  </si>
+  <si>
+    <t>0.4&gt;</t>
+  </si>
+  <si>
+    <t>[0.4</t>
+  </si>
+  <si>
+    <t>0.6&gt;</t>
+  </si>
+  <si>
+    <t>[0.6</t>
+  </si>
+  <si>
+    <t>0.8&gt;</t>
+  </si>
+  <si>
+    <t>[0.8</t>
+  </si>
+  <si>
+    <t>1]</t>
   </si>
 </sst>
 </file>
@@ -2309,13 +2339,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15837,10 +15867,10 @@
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B5" s="137">
+      <c r="B5" s="136">
         <v>1</v>
       </c>
-      <c r="C5" s="137" t="s">
+      <c r="C5" s="136" t="s">
         <v>378</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -15879,11 +15909,11 @@
         <v>INICIAL</v>
       </c>
       <c r="O5" s="46"/>
-      <c r="P5" s="135">
+      <c r="P5" s="137">
         <f>SUM(M5:M7)/3</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="136" t="str">
+      <c r="Q5" s="135" t="str">
         <f>IF(AND(P5&gt;=0.8,P5&lt;=1),"OPTIMIZADO",IF(AND(P5&gt;=0.6,P5&lt;0.8),"CUANTITATIVAMENTE GESTIONADO",IF(AND(P5&gt;=0.4,P5&lt;0.6),"DEFINIDO",IF(AND(P5&gt;=0.2,P5&lt;0.4),"ADMINISTRADO",IF(AND(P5&gt;=0,P5&lt;0.2),"INICIAL","Ingrese un valor válido")))))</f>
         <v>INICIAL</v>
       </c>
@@ -15897,8 +15927,8 @@
       </c>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B6" s="137"/>
-      <c r="C6" s="137"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="136"/>
       <c r="D6" s="1" t="s">
         <v>74</v>
       </c>
@@ -15935,12 +15965,12 @@
         <v>INICIAL</v>
       </c>
       <c r="O6" s="46"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="136"/>
+      <c r="P6" s="137"/>
+      <c r="Q6" s="135"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B7" s="137"/>
-      <c r="C7" s="137"/>
+      <c r="B7" s="136"/>
+      <c r="C7" s="136"/>
       <c r="D7" s="1" t="s">
         <v>87</v>
       </c>
@@ -15977,8 +16007,8 @@
         <v>INICIAL</v>
       </c>
       <c r="O7" s="46"/>
-      <c r="P7" s="135"/>
-      <c r="Q7" s="136"/>
+      <c r="P7" s="137"/>
+      <c r="Q7" s="135"/>
       <c r="S7" s="1"/>
       <c r="T7" s="59" t="s">
         <v>32</v>
@@ -16024,10 +16054,10 @@
       <c r="AA8" s="51"/>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B9" s="137">
+      <c r="B9" s="136">
         <v>2</v>
       </c>
-      <c r="C9" s="137" t="s">
+      <c r="C9" s="136" t="s">
         <v>380</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -16066,11 +16096,11 @@
         <v>INICIAL</v>
       </c>
       <c r="O9" s="46"/>
-      <c r="P9" s="135">
+      <c r="P9" s="137">
         <f>SUM(M9:M11)/3</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="136" t="str">
+      <c r="Q9" s="135" t="str">
         <f>IF(AND(P9&gt;=0.8,P9&lt;=1),"OPTIMIZADO",IF(AND(P9&gt;=0.6,P9&lt;0.8),"CUANTITATIVAMENTE GESTIONADO",IF(AND(P9&gt;=0.4,P9&lt;0.6),"DEFINIDO",IF(AND(P9&gt;=0.2,P9&lt;0.4),"ADMINISTRADO",IF(AND(P9&gt;=0,P9&lt;0.2),"INICIAL","Ingrese un valor válido")))))</f>
         <v>INICIAL</v>
       </c>
@@ -16098,8 +16128,8 @@
       <c r="AA9" s="51"/>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B10" s="137"/>
-      <c r="C10" s="137"/>
+      <c r="B10" s="136"/>
+      <c r="C10" s="136"/>
       <c r="D10" s="1" t="s">
         <v>74</v>
       </c>
@@ -16136,8 +16166,8 @@
         <v>INICIAL</v>
       </c>
       <c r="O10" s="46"/>
-      <c r="P10" s="135"/>
-      <c r="Q10" s="136"/>
+      <c r="P10" s="137"/>
+      <c r="Q10" s="135"/>
       <c r="S10" s="59" t="s">
         <v>87</v>
       </c>
@@ -16162,8 +16192,8 @@
       <c r="AA10" s="51"/>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B11" s="137"/>
-      <c r="C11" s="137"/>
+      <c r="B11" s="136"/>
+      <c r="C11" s="136"/>
       <c r="D11" s="1" t="s">
         <v>87</v>
       </c>
@@ -16200,8 +16230,8 @@
         <v>INICIAL</v>
       </c>
       <c r="O11" s="46"/>
-      <c r="P11" s="135"/>
-      <c r="Q11" s="136"/>
+      <c r="P11" s="137"/>
+      <c r="Q11" s="135"/>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.35">
       <c r="H12" s="97"/>
@@ -16212,10 +16242,10 @@
       <c r="Q12" s="45"/>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B13" s="137">
+      <c r="B13" s="136">
         <v>3</v>
       </c>
-      <c r="C13" s="137" t="s">
+      <c r="C13" s="136" t="s">
         <v>381</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -16254,18 +16284,18 @@
         <v>INICIAL</v>
       </c>
       <c r="O13" s="46"/>
-      <c r="P13" s="135">
+      <c r="P13" s="137">
         <f>SUM(M13:M15)/3</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="136" t="str">
+      <c r="Q13" s="135" t="str">
         <f>IF(AND(P13&gt;=0.8,P13&lt;=1),"OPTIMIZADO",IF(AND(P13&gt;=0.6,P13&lt;0.8),"CUANTITATIVAMENTE GESTIONADO",IF(AND(P13&gt;=0.4,P13&lt;0.6),"DEFINIDO",IF(AND(P13&gt;=0.2,P13&lt;0.4),"ADMINISTRADO",IF(AND(P13&gt;=0,P13&lt;0.2),"INICIAL","Ingrese un valor válido")))))</f>
         <v>INICIAL</v>
       </c>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B14" s="137"/>
-      <c r="C14" s="137"/>
+      <c r="B14" s="136"/>
+      <c r="C14" s="136"/>
       <c r="D14" s="1" t="s">
         <v>74</v>
       </c>
@@ -16302,12 +16332,12 @@
         <v>INICIAL</v>
       </c>
       <c r="O14" s="46"/>
-      <c r="P14" s="135"/>
-      <c r="Q14" s="136"/>
+      <c r="P14" s="137"/>
+      <c r="Q14" s="135"/>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B15" s="137"/>
-      <c r="C15" s="137"/>
+      <c r="B15" s="136"/>
+      <c r="C15" s="136"/>
       <c r="D15" s="1" t="s">
         <v>87</v>
       </c>
@@ -16344,8 +16374,8 @@
         <v>INICIAL</v>
       </c>
       <c r="O15" s="46"/>
-      <c r="P15" s="135"/>
-      <c r="Q15" s="136"/>
+      <c r="P15" s="137"/>
+      <c r="Q15" s="135"/>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.35">
       <c r="H16" s="97"/>
@@ -16356,10 +16386,10 @@
       <c r="Q16" s="45"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B17" s="137">
+      <c r="B17" s="136">
         <v>4</v>
       </c>
-      <c r="C17" s="137" t="s">
+      <c r="C17" s="136" t="s">
         <v>382</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -16398,18 +16428,18 @@
         <v>INICIAL</v>
       </c>
       <c r="O17" s="46"/>
-      <c r="P17" s="135">
+      <c r="P17" s="137">
         <f>SUM(M17:M19)/3</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="136" t="str">
+      <c r="Q17" s="135" t="str">
         <f>IF(AND(P17&gt;=0.8,P17&lt;=1),"OPTIMIZADO",IF(AND(P17&gt;=0.6,P17&lt;0.8),"CUANTITATIVAMENTE GESTIONADO",IF(AND(P17&gt;=0.4,P17&lt;0.6),"DEFINIDO",IF(AND(P17&gt;=0.2,P17&lt;0.4),"ADMINISTRADO",IF(AND(P17&gt;=0,P17&lt;0.2),"INICIAL","Ingrese un valor válido")))))</f>
         <v>INICIAL</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B18" s="137"/>
-      <c r="C18" s="137"/>
+      <c r="B18" s="136"/>
+      <c r="C18" s="136"/>
       <c r="D18" s="1" t="s">
         <v>74</v>
       </c>
@@ -16446,12 +16476,12 @@
         <v>INICIAL</v>
       </c>
       <c r="O18" s="46"/>
-      <c r="P18" s="135"/>
-      <c r="Q18" s="136"/>
+      <c r="P18" s="137"/>
+      <c r="Q18" s="135"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B19" s="137"/>
-      <c r="C19" s="137"/>
+      <c r="B19" s="136"/>
+      <c r="C19" s="136"/>
       <c r="D19" s="1" t="s">
         <v>87</v>
       </c>
@@ -16488,8 +16518,8 @@
         <v>INICIAL</v>
       </c>
       <c r="O19" s="46"/>
-      <c r="P19" s="135"/>
-      <c r="Q19" s="136"/>
+      <c r="P19" s="137"/>
+      <c r="Q19" s="135"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.35">
       <c r="H20" s="97"/>
@@ -16500,10 +16530,10 @@
       <c r="Q20" s="45"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B21" s="137">
+      <c r="B21" s="136">
         <v>5</v>
       </c>
-      <c r="C21" s="137" t="s">
+      <c r="C21" s="136" t="s">
         <v>383</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -16542,18 +16572,18 @@
         <v>INICIAL</v>
       </c>
       <c r="O21" s="46"/>
-      <c r="P21" s="135">
+      <c r="P21" s="137">
         <f>SUM(M21:M23)/3</f>
         <v>0</v>
       </c>
-      <c r="Q21" s="136" t="str">
+      <c r="Q21" s="135" t="str">
         <f>IF(AND(P21&gt;=0.8,P21&lt;=1),"OPTIMIZADO",IF(AND(P21&gt;=0.6,P21&lt;0.8),"CUANTITATIVAMENTE GESTIONADO",IF(AND(P21&gt;=0.4,P21&lt;0.6),"DEFINIDO",IF(AND(P21&gt;=0.2,P21&lt;0.4),"ADMINISTRADO",IF(AND(P21&gt;=0,P21&lt;0.2),"INICIAL","Ingrese un valor válido")))))</f>
         <v>INICIAL</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B22" s="137"/>
-      <c r="C22" s="137"/>
+      <c r="B22" s="136"/>
+      <c r="C22" s="136"/>
       <c r="D22" s="1" t="s">
         <v>74</v>
       </c>
@@ -16590,15 +16620,15 @@
         <v>INICIAL</v>
       </c>
       <c r="O22" s="46"/>
-      <c r="P22" s="135"/>
-      <c r="Q22" s="136"/>
+      <c r="P22" s="137"/>
+      <c r="Q22" s="135"/>
       <c r="S22" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B23" s="137"/>
-      <c r="C23" s="137"/>
+      <c r="B23" s="136"/>
+      <c r="C23" s="136"/>
       <c r="D23" s="1" t="s">
         <v>87</v>
       </c>
@@ -16635,8 +16665,8 @@
         <v>INICIAL</v>
       </c>
       <c r="O23" s="46"/>
-      <c r="P23" s="135"/>
-      <c r="Q23" s="136"/>
+      <c r="P23" s="137"/>
+      <c r="Q23" s="135"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.35">
       <c r="H24" s="97"/>
@@ -16647,10 +16677,10 @@
       <c r="Q24" s="45"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B25" s="137">
+      <c r="B25" s="136">
         <v>6</v>
       </c>
-      <c r="C25" s="137" t="s">
+      <c r="C25" s="136" t="s">
         <v>385</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -16689,18 +16719,18 @@
         <v>INICIAL</v>
       </c>
       <c r="O25" s="46"/>
-      <c r="P25" s="135">
+      <c r="P25" s="137">
         <f>SUM(M25:M27)/3</f>
         <v>0</v>
       </c>
-      <c r="Q25" s="136" t="str">
+      <c r="Q25" s="135" t="str">
         <f>IF(AND(P25&gt;=0.8,P25&lt;=1),"OPTIMIZADO",IF(AND(P25&gt;=0.6,P25&lt;0.8),"CUANTITATIVAMENTE GESTIONADO",IF(AND(P25&gt;=0.4,P25&lt;0.6),"DEFINIDO",IF(AND(P25&gt;=0.2,P25&lt;0.4),"ADMINISTRADO",IF(AND(P25&gt;=0,P25&lt;0.2),"INICIAL","Ingrese un valor válido")))))</f>
         <v>INICIAL</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B26" s="137"/>
-      <c r="C26" s="137"/>
+      <c r="B26" s="136"/>
+      <c r="C26" s="136"/>
       <c r="D26" s="1" t="s">
         <v>74</v>
       </c>
@@ -16737,12 +16767,12 @@
         <v>INICIAL</v>
       </c>
       <c r="O26" s="46"/>
-      <c r="P26" s="135"/>
-      <c r="Q26" s="136"/>
+      <c r="P26" s="137"/>
+      <c r="Q26" s="135"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B27" s="137"/>
-      <c r="C27" s="137"/>
+      <c r="B27" s="136"/>
+      <c r="C27" s="136"/>
       <c r="D27" s="1" t="s">
         <v>87</v>
       </c>
@@ -16779,8 +16809,8 @@
         <v>INICIAL</v>
       </c>
       <c r="O27" s="46"/>
-      <c r="P27" s="135"/>
-      <c r="Q27" s="136"/>
+      <c r="P27" s="137"/>
+      <c r="Q27" s="135"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.35">
       <c r="M28" s="45"/>
@@ -16797,11 +16827,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Q5:Q7"/>
-    <mergeCell ref="Q9:Q11"/>
-    <mergeCell ref="Q13:Q15"/>
-    <mergeCell ref="Q17:Q19"/>
-    <mergeCell ref="Q21:Q23"/>
+    <mergeCell ref="P5:P7"/>
+    <mergeCell ref="P9:P11"/>
+    <mergeCell ref="P13:P15"/>
+    <mergeCell ref="P17:P19"/>
+    <mergeCell ref="P21:P23"/>
     <mergeCell ref="Q25:Q27"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="C13:C15"/>
@@ -16818,11 +16848,11 @@
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="C25:C27"/>
     <mergeCell ref="P25:P27"/>
-    <mergeCell ref="P5:P7"/>
-    <mergeCell ref="P9:P11"/>
-    <mergeCell ref="P13:P15"/>
-    <mergeCell ref="P17:P19"/>
-    <mergeCell ref="P21:P23"/>
+    <mergeCell ref="Q5:Q7"/>
+    <mergeCell ref="Q9:Q11"/>
+    <mergeCell ref="Q13:Q15"/>
+    <mergeCell ref="Q17:Q19"/>
+    <mergeCell ref="Q21:Q23"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:H27">
     <cfRule type="iconSet" priority="41">
@@ -17949,8 +17979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1262A127-4DF6-4F4F-B8F9-B35F9ACD5893}">
   <dimension ref="B2:J11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="E6:F6"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18023,11 +18053,11 @@
       <c r="D6" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="42">
-        <v>0</v>
-      </c>
-      <c r="F6" s="42">
-        <v>0.2</v>
+      <c r="E6" s="42" t="s">
+        <v>441</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="29" x14ac:dyDescent="0.35">
@@ -18040,11 +18070,11 @@
       <c r="D7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="42">
-        <v>0.2</v>
-      </c>
-      <c r="F7" s="42">
-        <v>0.4</v>
+      <c r="E7" s="42" t="s">
+        <v>443</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="29" x14ac:dyDescent="0.35">
@@ -18057,11 +18087,11 @@
       <c r="D8" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="42">
-        <v>0.4</v>
-      </c>
-      <c r="F8" s="42">
-        <v>0.6</v>
+      <c r="E8" s="42" t="s">
+        <v>445</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="58" x14ac:dyDescent="0.35">
@@ -18074,11 +18104,11 @@
       <c r="D9" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="42">
-        <v>0.6</v>
-      </c>
-      <c r="F9" s="42">
-        <v>0.8</v>
+      <c r="E9" s="42" t="s">
+        <v>447</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="58" x14ac:dyDescent="0.35">
@@ -18091,11 +18121,11 @@
       <c r="D10" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="F10" s="42">
-        <v>1</v>
+      <c r="E10" s="42" t="s">
+        <v>449</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.35">
@@ -20560,26 +20590,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c3e8fa33-f11c-4432-b9aa-f669a142e5ce">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8dceb93e-2434-4a2d-9950-ee586c124d8b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B4690A5B055F5C409484550C3CDF1530" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="d0d7474e99d73ad900a7c2e7df9a3823">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c3e8fa33-f11c-4432-b9aa-f669a142e5ce" xmlns:ns3="8dceb93e-2434-4a2d-9950-ee586c124d8b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="21a22197c1f37d77da14d9d70acf3e32" ns2:_="" ns3:_="">
     <xsd:import namespace="c3e8fa33-f11c-4432-b9aa-f669a142e5ce"/>
@@ -20768,26 +20778,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68BACD7B-8447-493C-BF6E-C56F6B779E95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c3e8fa33-f11c-4432-b9aa-f669a142e5ce"/>
-    <ds:schemaRef ds:uri="8dceb93e-2434-4a2d-9950-ee586c124d8b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEE29674-FA7B-4C11-BF57-A50C5AA76FD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c3e8fa33-f11c-4432-b9aa-f669a142e5ce">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8dceb93e-2434-4a2d-9950-ee586c124d8b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E55D8DF-D3BE-41BE-8E95-979850F179B7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20804,4 +20815,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEE29674-FA7B-4C11-BF57-A50C5AA76FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68BACD7B-8447-493C-BF6E-C56F6B779E95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c3e8fa33-f11c-4432-b9aa-f669a142e5ce"/>
+    <ds:schemaRef ds:uri="8dceb93e-2434-4a2d-9950-ee586c124d8b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>